<commit_message>
user stories en layout
Meer user stories afgerond en layout aangepast
</commit_message>
<xml_diff>
--- a/DOCUMENTATIE/userStories.xlsx
+++ b/DOCUMENTATIE/userStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damhe\Documents\maschool\bewijzenmap\periode2.1\BAP\bap-website\DOCUMENTATIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75FC9E07-9FFB-47EC-9211-1F6CDE81944E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A31BA-8088-4BAF-B398-466B27BBAF62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -1530,8 +1530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8C07C-95E6-5F45-AA16-00A7B9F9E844}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="94" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1701,7 +1701,7 @@
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>20</v>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>24</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>27</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>30</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>128</v>
@@ -2614,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3217D4F-5AF1-9F44-A8EF-7F34D2E586CC}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="53" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
404 pagina gemaakt, met db ge-oefend
</commit_message>
<xml_diff>
--- a/DOCUMENTATIE/userStories.xlsx
+++ b/DOCUMENTATIE/userStories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damhe\Documents\maschool\bewijzenmap\periode2.1\BAP\bap-website\DOCUMENTATIE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8A31BA-8088-4BAF-B398-466B27BBAF62}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F2A31D-0D34-4A50-A5AB-791DE2DEEFE2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{96E4F204-A96B-B442-B776-0E7F469FE00D}"/>
   </bookViews>
   <sheets>
     <sheet name="Basis" sheetId="1" r:id="rId1"/>
@@ -1530,7 +1530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F8C07C-95E6-5F45-AA16-00A7B9F9E844}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="78" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -2614,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3217D4F-5AF1-9F44-A8EF-7F34D2E586CC}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView zoomScale="53" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2855,7 +2855,7 @@
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>180</v>
@@ -3090,21 +3090,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F8D01017B67FFC40B6EAF835C0079E48" ma:contentTypeVersion="10" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="c7194cc31030e2712d76c2006e0d75af">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="584c6f05-645a-45c2-af5b-a2298cf6e1b5" xmlns:ns3="5c2aeaab-3434-48d9-b2ba-99c708216bcd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="420f24c0cdcfc5bd7329cba19e0bdf1c" ns2:_="" ns3:_="">
     <xsd:import namespace="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
@@ -3307,32 +3292,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
-    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C62A3BA8-675C-43E7-9E30-618B42A3DB6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3349,4 +3324,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2490BF6-BAD1-45FA-8E2E-1DC0E56639F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C4C429B-C437-4A37-B7CA-137886FFB6B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="5c2aeaab-3434-48d9-b2ba-99c708216bcd"/>
+    <ds:schemaRef ds:uri="584c6f05-645a-45c2-af5b-a2298cf6e1b5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>